<commit_message>
Week 6 and Week 7 updates
</commit_message>
<xml_diff>
--- a/Week7/dictionary/sal2021_is.new.xlsx
+++ b/Week7/dictionary/sal2021_is.new.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10818"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10828"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidtorres/Code/NU/TIM7020/Week6/dictionary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidtorres/Code/NU/TIM7020/Week7/dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CB2626-FF41-D94E-ACE4-2FA1CA19A29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C22DF5-A5F9-0D48-B534-0DCC84094E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40840" yWindow="2000" windowWidth="27080" windowHeight="21500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="234">
   <si>
     <t>varnumber</t>
   </si>
@@ -1088,7 +1088,7 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1165,6 +1165,9 @@
       <c r="E3" t="s">
         <v>15</v>
       </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
       <c r="G3" t="s">
         <v>16</v>
       </c>

</xml_diff>